<commit_message>
Ajout de INTERNALVALUE dans PARAM_LIST_ALLOWED
</commit_message>
<xml_diff>
--- a/TNR_JDD/JDD.RT.EQU.xlsx
+++ b/TNR_JDD/JDD.RT.EQU.xlsx
@@ -16,7 +16,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId12" roundtripDataChecksum="/M0aYMYJNav7HCqAtE9Wd0DpJO2+PtLi9Uf9Lco8U7E="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId12" roundtripDataChecksum="mVmwD/d4aAsSIcH7m/gtYXJNc7weRfadBTRA5BHXFJQ="/>
     </ext>
   </extLst>
 </workbook>
@@ -114,14 +114,14 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mjEy+UuCFMd3I95eEnXFIwLqv4BzA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mjK/gRnrXUkH4k+J4VcGz9/gtmp+w=="/>
     </ext>
   </extLst>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="291">
   <si>
     <t>Date</t>
   </si>
@@ -754,6 +754,15 @@
   </si>
   <si>
     <t>FOREIGNKEY</t>
+  </si>
+  <si>
+    <t>ID_NUMEMP*EMP*ST_CODCOU</t>
+  </si>
+  <si>
+    <t>INTERNALVALUE</t>
+  </si>
+  <si>
+    <t>GROUPE</t>
   </si>
   <si>
     <t>SEQUENCE</t>
@@ -1470,7 +1479,9 @@
     <xf borderId="0" fillId="10" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="15" fontId="7" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="15" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="5" fillId="6" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="5" fillId="16" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
   </cellXfs>
@@ -5079,10 +5090,10 @@
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1.0" ySplit="6.0" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1.0" ySplit="7.0" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1" pane="topRight"/>
-      <selection activeCell="A7" sqref="A7" pane="bottomLeft"/>
-      <selection activeCell="B7" sqref="B7" pane="bottomRight"/>
+      <selection activeCell="A8" sqref="A8" pane="bottomLeft"/>
+      <selection activeCell="B8" sqref="B8" pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
@@ -5100,7 +5111,7 @@
     <col customWidth="1" min="15" max="15" width="24.13"/>
     <col customWidth="1" min="16" max="16" width="14.38"/>
     <col customWidth="1" min="19" max="19" width="27.0"/>
-    <col customWidth="1" min="21" max="21" width="24.63"/>
+    <col customWidth="1" min="21" max="21" width="11.13"/>
     <col customWidth="1" min="22" max="22" width="13.88"/>
     <col customWidth="1" min="25" max="25" width="24.88"/>
     <col customWidth="1" min="27" max="27" width="20.75"/>
@@ -5523,8 +5534,8 @@
       <c r="C3" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="40" t="s">
-        <v>9</v>
+      <c r="D3" s="41" t="s">
+        <v>205</v>
       </c>
       <c r="E3" s="40" t="s">
         <v>9</v>
@@ -5574,9 +5585,7 @@
       <c r="T3" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="U3" s="40" t="s">
-        <v>9</v>
-      </c>
+      <c r="U3" s="41"/>
       <c r="V3" s="40" t="s">
         <v>9</v>
       </c>
@@ -5717,209 +5726,81 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="40" t="s">
-        <v>205</v>
-      </c>
-      <c r="B4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="40" t="s">
-        <v>9</v>
-      </c>
+      <c r="A4" s="41" t="s">
+        <v>206</v>
+      </c>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
       <c r="D4" s="40"/>
-      <c r="E4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="J4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="K4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="L4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="M4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="N4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="O4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="P4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="R4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="S4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="T4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="U4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="V4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="W4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="X4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="AD4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="AE4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="AF4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="AG4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="AH4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="AI4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="AJ4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="AK4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="AL4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="AM4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="AN4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="AO4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="AP4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="AQ4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="AR4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="AS4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="AT4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="AU4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="AV4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="AW4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="AX4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="AY4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="AZ4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="BA4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="BB4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="BC4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="BD4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="BE4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="BF4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="BG4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="BH4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="BI4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="BJ4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="BK4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="BL4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="BM4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="BN4" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="BO4" s="40" t="s">
-        <v>9</v>
-      </c>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="40"/>
+      <c r="P4" s="40"/>
+      <c r="Q4" s="40"/>
+      <c r="R4" s="40"/>
+      <c r="S4" s="40"/>
+      <c r="T4" s="40"/>
+      <c r="U4" s="41" t="s">
+        <v>207</v>
+      </c>
+      <c r="V4" s="40"/>
+      <c r="W4" s="40"/>
+      <c r="X4" s="40"/>
+      <c r="Y4" s="40"/>
+      <c r="Z4" s="40"/>
+      <c r="AA4" s="40"/>
+      <c r="AB4" s="40"/>
+      <c r="AC4" s="40"/>
+      <c r="AD4" s="40"/>
+      <c r="AE4" s="40"/>
+      <c r="AF4" s="40"/>
+      <c r="AG4" s="40"/>
+      <c r="AH4" s="40"/>
+      <c r="AI4" s="40"/>
+      <c r="AJ4" s="40"/>
+      <c r="AK4" s="40"/>
+      <c r="AL4" s="40"/>
+      <c r="AM4" s="40"/>
+      <c r="AN4" s="40"/>
+      <c r="AO4" s="40"/>
+      <c r="AP4" s="40"/>
+      <c r="AQ4" s="40"/>
+      <c r="AR4" s="40"/>
+      <c r="AS4" s="40"/>
+      <c r="AT4" s="40"/>
+      <c r="AU4" s="40"/>
+      <c r="AV4" s="40"/>
+      <c r="AW4" s="40"/>
+      <c r="AX4" s="40"/>
+      <c r="AY4" s="40"/>
+      <c r="AZ4" s="40"/>
+      <c r="BA4" s="40"/>
+      <c r="BB4" s="40"/>
+      <c r="BC4" s="40"/>
+      <c r="BD4" s="40"/>
+      <c r="BE4" s="40"/>
+      <c r="BF4" s="40"/>
+      <c r="BG4" s="40"/>
+      <c r="BH4" s="40"/>
+      <c r="BI4" s="40"/>
+      <c r="BJ4" s="40"/>
+      <c r="BK4" s="40"/>
+      <c r="BL4" s="40"/>
+      <c r="BM4" s="40"/>
+      <c r="BN4" s="40"/>
+      <c r="BO4" s="40"/>
     </row>
     <row r="5">
       <c r="A5" s="40" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B5" s="40" t="s">
         <v>9</v>
@@ -5927,11 +5808,9 @@
       <c r="C5" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="40" t="s">
-        <v>9</v>
-      </c>
+      <c r="D5" s="40"/>
       <c r="E5" s="40" t="s">
-        <v>207</v>
+        <v>9</v>
       </c>
       <c r="F5" s="40" t="s">
         <v>9</v>
@@ -5961,7 +5840,7 @@
         <v>9</v>
       </c>
       <c r="O5" s="40" t="s">
-        <v>207</v>
+        <v>9</v>
       </c>
       <c r="P5" s="40" t="s">
         <v>9</v>
@@ -5973,7 +5852,7 @@
         <v>9</v>
       </c>
       <c r="S5" s="40" t="s">
-        <v>207</v>
+        <v>9</v>
       </c>
       <c r="T5" s="40" t="s">
         <v>9</v>
@@ -6006,13 +5885,13 @@
         <v>9</v>
       </c>
       <c r="AD5" s="40" t="s">
-        <v>207</v>
+        <v>9</v>
       </c>
       <c r="AE5" s="40" t="s">
         <v>9</v>
       </c>
       <c r="AF5" s="40" t="s">
-        <v>207</v>
+        <v>9</v>
       </c>
       <c r="AG5" s="40" t="s">
         <v>9</v>
@@ -6048,7 +5927,7 @@
         <v>9</v>
       </c>
       <c r="AR5" s="40" t="s">
-        <v>207</v>
+        <v>9</v>
       </c>
       <c r="AS5" s="40" t="s">
         <v>9</v>
@@ -6057,7 +5936,7 @@
         <v>9</v>
       </c>
       <c r="AU5" s="40" t="s">
-        <v>208</v>
+        <v>9</v>
       </c>
       <c r="AV5" s="40" t="s">
         <v>9</v>
@@ -6090,1010 +5969,1080 @@
         <v>9</v>
       </c>
       <c r="BF5" s="40" t="s">
-        <v>207</v>
+        <v>9</v>
       </c>
       <c r="BG5" s="40" t="s">
         <v>9</v>
       </c>
       <c r="BH5" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="BI5" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="BJ5" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="BK5" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="BL5" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="BM5" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="BN5" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="BO5" s="40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="40" t="s">
         <v>209</v>
       </c>
-      <c r="BI5" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="BJ5" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="BK5" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="BL5" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="BM5" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="BN5" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="BO5" s="40" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="42" t="s">
+      <c r="B6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="40" t="s">
         <v>210</v>
       </c>
-      <c r="B6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="I6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="J6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="K6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="L6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="M6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="N6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="O6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="P6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="R6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="S6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="T6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="U6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="V6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="W6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="X6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="AD6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="AE6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="AF6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="AG6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="AH6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="AI6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="AJ6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="AK6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="AL6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="AM6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="AN6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="AO6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="AP6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="AQ6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="AR6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="AS6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="AT6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="AU6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="AV6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="AW6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="AX6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="AY6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="AZ6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="BA6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="BB6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="BC6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="BD6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="BE6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="BF6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="BG6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="BH6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="BI6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="BJ6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="BK6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="BL6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="BM6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="BN6" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="BO6" s="42" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="43" t="s">
+      <c r="F6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="M6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="N6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="O6" s="40" t="s">
+        <v>210</v>
+      </c>
+      <c r="P6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="R6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="S6" s="40" t="s">
+        <v>210</v>
+      </c>
+      <c r="T6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="U6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="V6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="W6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="X6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD6" s="40" t="s">
+        <v>210</v>
+      </c>
+      <c r="AE6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF6" s="40" t="s">
+        <v>210</v>
+      </c>
+      <c r="AG6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="AI6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="AJ6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="AK6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="AL6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="AM6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="AN6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="AO6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="AP6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="AQ6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="AR6" s="40" t="s">
+        <v>210</v>
+      </c>
+      <c r="AS6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="AT6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="AU6" s="40" t="s">
         <v>211</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="AV6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="AW6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="AX6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="AY6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="AZ6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="BA6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="BB6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="BC6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="BD6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="BE6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="BF6" s="40" t="s">
+        <v>210</v>
+      </c>
+      <c r="BG6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="BH6" s="40" t="s">
         <v>212</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="BI6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="BJ6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="BK6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="BL6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="BM6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="BN6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="BO6" s="40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="42" t="s">
         <v>213</v>
       </c>
-      <c r="D7" s="19" t="s">
-        <v>214</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>215</v>
-      </c>
-      <c r="F7" s="45" t="s">
-        <v>216</v>
-      </c>
-      <c r="G7" s="45" t="s">
-        <v>216</v>
-      </c>
-      <c r="H7" s="32" t="s">
-        <v>216</v>
-      </c>
-      <c r="I7" s="32" t="s">
-        <v>216</v>
-      </c>
-      <c r="J7" s="46" t="s">
-        <v>212</v>
-      </c>
-      <c r="K7" s="46" t="s">
-        <v>212</v>
-      </c>
-      <c r="L7" s="47" t="s">
-        <v>217</v>
-      </c>
-      <c r="M7" s="46" t="s">
-        <v>212</v>
-      </c>
-      <c r="N7" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="O7" s="19" t="s">
-        <v>218</v>
-      </c>
-      <c r="P7" s="47" t="s">
-        <v>217</v>
-      </c>
-      <c r="Q7" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="R7" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="S7" s="19" t="s">
-        <v>219</v>
-      </c>
-      <c r="T7" s="21">
-        <v>0.0</v>
-      </c>
-      <c r="U7" s="25" t="s">
-        <v>220</v>
-      </c>
-      <c r="V7" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="W7" s="21">
-        <v>1.0</v>
-      </c>
-      <c r="X7" s="21">
-        <v>1.0</v>
-      </c>
-      <c r="Y7" s="18" t="str">
-        <f t="shared" ref="Y7:Y9" si="1">CONCATENATE(UPPER(AA7),REPT(".",30-LEN(AA7)))</f>
-        <v>EQU.RT.EQU.001.CRE.01.........</v>
-      </c>
-      <c r="Z7" s="19" t="s">
-        <v>222</v>
-      </c>
-      <c r="AA7" s="19" t="s">
-        <v>223</v>
-      </c>
-      <c r="AB7" s="19">
-        <v>1000.0</v>
-      </c>
-      <c r="AC7" s="19">
-        <v>10.0</v>
-      </c>
-      <c r="AD7" s="19">
-        <v>110.0</v>
-      </c>
-      <c r="AE7" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="AF7" s="19" t="s">
-        <v>220</v>
-      </c>
-      <c r="AG7" s="19" t="s">
-        <v>224</v>
-      </c>
-      <c r="AH7" s="19" t="s">
-        <v>225</v>
-      </c>
-      <c r="AI7" s="19" t="s">
-        <v>226</v>
-      </c>
-      <c r="AJ7" s="19" t="s">
-        <v>227</v>
-      </c>
-      <c r="AK7" s="48">
-        <v>44920.0</v>
-      </c>
-      <c r="AL7" s="19">
-        <v>10000.0</v>
-      </c>
-      <c r="AM7" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="AN7" s="19" t="s">
-        <v>228</v>
-      </c>
-      <c r="AO7" s="48">
-        <v>45651.0</v>
-      </c>
-      <c r="AP7" s="19">
-        <v>10000.0</v>
-      </c>
-      <c r="AQ7" s="19" t="s">
-        <v>229</v>
-      </c>
-      <c r="AR7" s="19" t="s">
-        <v>229</v>
-      </c>
-      <c r="AS7" s="19" t="s">
-        <v>229</v>
-      </c>
-      <c r="AT7" s="49" t="str">
-        <f t="shared" ref="AT7:AT9" si="2">Y7</f>
-        <v>EQU.RT.EQU.001.CRE.01.........</v>
-      </c>
-      <c r="AU7" s="19" t="s">
-        <v>230</v>
-      </c>
-      <c r="AV7" s="19" t="s">
-        <v>229</v>
-      </c>
-      <c r="AW7" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="AX7" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="AY7" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="AZ7" s="47" t="s">
-        <v>231</v>
-      </c>
-      <c r="BA7" s="19">
-        <v>100000.0</v>
-      </c>
-      <c r="BB7" s="48">
-        <v>49303.0</v>
-      </c>
-      <c r="BC7" s="19">
-        <v>1000000.0</v>
-      </c>
-      <c r="BD7" s="19" t="s">
-        <v>230</v>
-      </c>
-      <c r="BE7" s="19">
-        <v>1.0</v>
-      </c>
-      <c r="BF7" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="BG7" s="48">
-        <v>44920.0</v>
-      </c>
-      <c r="BH7" s="25" t="s">
-        <v>232</v>
-      </c>
-      <c r="BI7" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="BJ7" s="19">
-        <v>1000.0</v>
-      </c>
-      <c r="BK7" s="19" t="s">
-        <v>233</v>
-      </c>
-      <c r="BL7" s="50" t="s">
-        <v>231</v>
-      </c>
-      <c r="BM7" s="50" t="s">
-        <v>231</v>
-      </c>
-      <c r="BN7" s="50" t="s">
-        <v>234</v>
-      </c>
-      <c r="BO7" s="50" t="s">
-        <v>234</v>
+      <c r="B7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="K7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="L7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="M7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="N7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="O7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="P7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="R7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="S7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="T7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="U7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="V7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="W7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="X7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="AI7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="AJ7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="AK7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="AL7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="AM7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="AN7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="AO7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="AP7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="AQ7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="AR7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="AS7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="AT7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="AU7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="AV7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="AW7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="AX7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="AY7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="AZ7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="BA7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="BB7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="BC7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="BD7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="BE7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="BF7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="BG7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="BH7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="BI7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="BJ7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="BK7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="BL7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="BM7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="BN7" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="BO7" s="42" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="43" t="s">
-        <v>235</v>
-      </c>
-      <c r="B8" s="21">
-        <v>1000.0</v>
+        <v>214</v>
+      </c>
+      <c r="B8" s="44" t="s">
+        <v>215</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>237</v>
+        <v>217</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>238</v>
+        <v>218</v>
       </c>
       <c r="F8" s="45" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="G8" s="45" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="H8" s="32" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="I8" s="32" t="s">
-        <v>216</v>
-      </c>
-      <c r="J8" s="47">
-        <v>1000.0</v>
-      </c>
-      <c r="K8" s="47">
-        <v>2000.0</v>
-      </c>
-      <c r="L8" s="51" t="s">
-        <v>217</v>
-      </c>
-      <c r="M8" s="47">
-        <v>3000.0</v>
+        <v>219</v>
+      </c>
+      <c r="J8" s="46" t="s">
+        <v>215</v>
+      </c>
+      <c r="K8" s="46" t="s">
+        <v>215</v>
+      </c>
+      <c r="L8" s="47" t="s">
+        <v>220</v>
+      </c>
+      <c r="M8" s="46" t="s">
+        <v>215</v>
       </c>
       <c r="N8" s="19" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="O8" s="19" t="s">
-        <v>239</v>
-      </c>
-      <c r="P8" s="51" t="s">
-        <v>217</v>
+        <v>221</v>
+      </c>
+      <c r="P8" s="47" t="s">
+        <v>220</v>
       </c>
       <c r="Q8" s="19" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="R8" s="19" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="S8" s="19" t="s">
-        <v>240</v>
+        <v>222</v>
       </c>
       <c r="T8" s="21">
         <v>0.0</v>
       </c>
       <c r="U8" s="25" t="s">
-        <v>241</v>
+        <v>223</v>
       </c>
       <c r="V8" s="19" t="s">
-        <v>242</v>
+        <v>224</v>
       </c>
       <c r="W8" s="21">
         <v>1.0</v>
       </c>
       <c r="X8" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="Y8" s="18" t="str">
+        <f t="shared" ref="Y8:Y10" si="1">CONCATENATE(UPPER(AA8),REPT(".",30-LEN(AA8)))</f>
+        <v>EQU.RT.EQU.001.CRE.01.........</v>
+      </c>
+      <c r="Z8" s="19" t="s">
+        <v>225</v>
+      </c>
+      <c r="AA8" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="AB8" s="19">
+        <v>1000.0</v>
+      </c>
+      <c r="AC8" s="19">
+        <v>10.0</v>
+      </c>
+      <c r="AD8" s="19">
+        <v>110.0</v>
+      </c>
+      <c r="AE8" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="AF8" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="AG8" s="19" t="s">
+        <v>227</v>
+      </c>
+      <c r="AH8" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="AI8" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="AJ8" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="AK8" s="48">
+        <v>44920.0</v>
+      </c>
+      <c r="AL8" s="19">
+        <v>10000.0</v>
+      </c>
+      <c r="AM8" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="AN8" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="AO8" s="48">
+        <v>45651.0</v>
+      </c>
+      <c r="AP8" s="19">
+        <v>10000.0</v>
+      </c>
+      <c r="AQ8" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="AR8" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="AS8" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="AT8" s="49" t="str">
+        <f t="shared" ref="AT8:AT10" si="2">Y8</f>
+        <v>EQU.RT.EQU.001.CRE.01.........</v>
+      </c>
+      <c r="AU8" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="AV8" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="AW8" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="AX8" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="AY8" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="AZ8" s="47" t="s">
+        <v>234</v>
+      </c>
+      <c r="BA8" s="19">
+        <v>100000.0</v>
+      </c>
+      <c r="BB8" s="48">
+        <v>49303.0</v>
+      </c>
+      <c r="BC8" s="19">
+        <v>1000000.0</v>
+      </c>
+      <c r="BD8" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="BE8" s="19">
+        <v>1.0</v>
+      </c>
+      <c r="BF8" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="BG8" s="48">
+        <v>44920.0</v>
+      </c>
+      <c r="BH8" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="BI8" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="BJ8" s="19">
+        <v>1000.0</v>
+      </c>
+      <c r="BK8" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="BL8" s="50" t="s">
+        <v>234</v>
+      </c>
+      <c r="BM8" s="50" t="s">
+        <v>234</v>
+      </c>
+      <c r="BN8" s="50" t="s">
+        <v>237</v>
+      </c>
+      <c r="BO8" s="50" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" s="43" t="s">
+        <v>238</v>
+      </c>
+      <c r="B9" s="21">
+        <v>1000.0</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>239</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="F9" s="45" t="s">
+        <v>219</v>
+      </c>
+      <c r="G9" s="45" t="s">
+        <v>219</v>
+      </c>
+      <c r="H9" s="32" t="s">
+        <v>219</v>
+      </c>
+      <c r="I9" s="32" t="s">
+        <v>219</v>
+      </c>
+      <c r="J9" s="47">
+        <v>1000.0</v>
+      </c>
+      <c r="K9" s="47">
+        <v>2000.0</v>
+      </c>
+      <c r="L9" s="51" t="s">
+        <v>220</v>
+      </c>
+      <c r="M9" s="47">
+        <v>3000.0</v>
+      </c>
+      <c r="N9" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="O9" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="P9" s="51" t="s">
+        <v>220</v>
+      </c>
+      <c r="Q9" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="R9" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="S9" s="19" t="s">
+        <v>243</v>
+      </c>
+      <c r="T9" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="U9" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="V9" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="W9" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="X9" s="21">
         <v>2.0</v>
       </c>
-      <c r="Y8" s="18" t="str">
+      <c r="Y9" s="18" t="str">
         <f t="shared" si="1"/>
         <v>EQU.RT.EQU.001.LEC.01.........</v>
       </c>
-      <c r="Z8" s="19" t="s">
-        <v>243</v>
-      </c>
-      <c r="AA8" s="19" t="s">
+      <c r="Z9" s="19" t="s">
+        <v>246</v>
+      </c>
+      <c r="AA9" s="19" t="s">
+        <v>247</v>
+      </c>
+      <c r="AB9" s="19">
+        <v>1001.0</v>
+      </c>
+      <c r="AC9" s="19">
+        <v>20.0</v>
+      </c>
+      <c r="AD9" s="19">
+        <v>120.0</v>
+      </c>
+      <c r="AE9" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="AF9" s="19" t="s">
         <v>244</v>
       </c>
-      <c r="AB8" s="19">
-        <v>1001.0</v>
-      </c>
-      <c r="AC8" s="19">
-        <v>20.0</v>
-      </c>
-      <c r="AD8" s="19">
-        <v>120.0</v>
-      </c>
-      <c r="AE8" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="AF8" s="19" t="s">
-        <v>241</v>
-      </c>
-      <c r="AG8" s="19" t="s">
-        <v>245</v>
-      </c>
-      <c r="AH8" s="19" t="s">
-        <v>246</v>
-      </c>
-      <c r="AI8" s="19" t="s">
-        <v>247</v>
-      </c>
-      <c r="AJ8" s="19" t="s">
+      <c r="AG9" s="19" t="s">
         <v>248</v>
       </c>
-      <c r="AK8" s="52">
+      <c r="AH9" s="19" t="s">
+        <v>249</v>
+      </c>
+      <c r="AI9" s="19" t="s">
+        <v>250</v>
+      </c>
+      <c r="AJ9" s="19" t="s">
+        <v>251</v>
+      </c>
+      <c r="AK9" s="52">
         <v>43922.0</v>
       </c>
-      <c r="AL8" s="19">
+      <c r="AL9" s="19">
         <v>20000.0</v>
       </c>
-      <c r="AM8" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="AN8" s="19" t="s">
-        <v>249</v>
-      </c>
-      <c r="AO8" s="52">
+      <c r="AM9" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="AN9" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="AO9" s="52">
         <v>44652.0</v>
       </c>
-      <c r="AP8" s="19">
+      <c r="AP9" s="19">
         <v>20000.0</v>
       </c>
-      <c r="AQ8" s="19" t="s">
-        <v>230</v>
-      </c>
-      <c r="AR8" s="19" t="s">
-        <v>230</v>
-      </c>
-      <c r="AS8" s="19" t="s">
-        <v>230</v>
-      </c>
-      <c r="AT8" s="49" t="str">
+      <c r="AQ9" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="AR9" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="AS9" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="AT9" s="49" t="str">
         <f t="shared" si="2"/>
         <v>EQU.RT.EQU.001.LEC.01.........</v>
       </c>
-      <c r="AU8" s="19" t="s">
-        <v>230</v>
-      </c>
-      <c r="AV8" s="19" t="s">
-        <v>230</v>
-      </c>
-      <c r="AW8" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="AX8" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="AY8" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="AZ8" s="51" t="s">
-        <v>231</v>
-      </c>
-      <c r="BA8" s="19">
+      <c r="AU9" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="AV9" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="AW9" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="AX9" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="AY9" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="AZ9" s="51" t="s">
+        <v>234</v>
+      </c>
+      <c r="BA9" s="19">
         <v>110000.0</v>
       </c>
-      <c r="BB8" s="52">
+      <c r="BB9" s="52">
         <v>48305.0</v>
       </c>
-      <c r="BC8" s="19">
+      <c r="BC9" s="19">
         <v>2000000.0</v>
       </c>
-      <c r="BD8" s="19" t="s">
-        <v>229</v>
-      </c>
-      <c r="BE8" s="19">
+      <c r="BD9" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="BE9" s="19">
         <v>2.0</v>
       </c>
-      <c r="BF8" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="BG8" s="52">
+      <c r="BF9" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="BG9" s="52">
         <v>44652.0</v>
       </c>
-      <c r="BH8" s="25" t="s">
-        <v>232</v>
-      </c>
-      <c r="BI8" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="BJ8" s="19">
+      <c r="BH9" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="BI9" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="BJ9" s="19">
         <v>1001.0</v>
       </c>
-      <c r="BK8" s="19" t="s">
-        <v>250</v>
-      </c>
-      <c r="BL8" s="50" t="s">
-        <v>231</v>
-      </c>
-      <c r="BM8" s="50" t="s">
-        <v>231</v>
-      </c>
-      <c r="BN8" s="50" t="s">
+      <c r="BK9" s="19" t="s">
+        <v>253</v>
+      </c>
+      <c r="BL9" s="50" t="s">
         <v>234</v>
       </c>
-      <c r="BO8" s="50" t="s">
+      <c r="BM9" s="50" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="43" t="s">
-        <v>251</v>
-      </c>
-      <c r="B9" s="21">
+      <c r="BN9" s="50" t="s">
+        <v>237</v>
+      </c>
+      <c r="BO9" s="50" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="A10" s="43" t="s">
+        <v>254</v>
+      </c>
+      <c r="B10" s="21">
         <v>1001.0</v>
       </c>
-      <c r="C9" s="19" t="s">
-        <v>252</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>253</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>254</v>
-      </c>
-      <c r="F9" s="45" t="s">
-        <v>216</v>
-      </c>
-      <c r="G9" s="45" t="s">
-        <v>216</v>
-      </c>
-      <c r="H9" s="32" t="s">
-        <v>216</v>
-      </c>
-      <c r="I9" s="32" t="s">
-        <v>216</v>
-      </c>
-      <c r="J9" s="47">
+      <c r="C10" s="19" t="s">
+        <v>255</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>256</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>257</v>
+      </c>
+      <c r="F10" s="45" t="s">
+        <v>219</v>
+      </c>
+      <c r="G10" s="45" t="s">
+        <v>219</v>
+      </c>
+      <c r="H10" s="32" t="s">
+        <v>219</v>
+      </c>
+      <c r="I10" s="32" t="s">
+        <v>219</v>
+      </c>
+      <c r="J10" s="47">
         <v>1001.0</v>
       </c>
-      <c r="K9" s="47">
+      <c r="K10" s="47">
         <v>2001.0</v>
       </c>
-      <c r="L9" s="51" t="s">
-        <v>217</v>
-      </c>
-      <c r="M9" s="47">
+      <c r="L10" s="51" t="s">
+        <v>220</v>
+      </c>
+      <c r="M10" s="47">
         <v>3001.0</v>
       </c>
-      <c r="N9" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="O9" s="19" t="s">
-        <v>255</v>
-      </c>
-      <c r="P9" s="51" t="s">
-        <v>217</v>
-      </c>
-      <c r="Q9" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="R9" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="S9" s="19" t="s">
-        <v>256</v>
-      </c>
-      <c r="T9" s="21">
+      <c r="N10" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="O10" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="P10" s="51" t="s">
+        <v>220</v>
+      </c>
+      <c r="Q10" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="R10" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="S10" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="T10" s="21">
         <v>0.0</v>
       </c>
-      <c r="U9" s="25" t="s">
-        <v>257</v>
-      </c>
-      <c r="V9" s="19" t="s">
-        <v>258</v>
-      </c>
-      <c r="W9" s="21">
+      <c r="U10" s="25" t="s">
+        <v>260</v>
+      </c>
+      <c r="V10" s="19" t="s">
+        <v>261</v>
+      </c>
+      <c r="W10" s="21">
         <v>1.0</v>
       </c>
-      <c r="X9" s="21">
+      <c r="X10" s="21">
         <v>3.0</v>
       </c>
-      <c r="Y9" s="18" t="str">
+      <c r="Y10" s="18" t="str">
         <f t="shared" si="1"/>
         <v>EQU.RT.EQU.001.MAJ.01.........</v>
       </c>
-      <c r="Z9" s="19" t="s">
-        <v>259</v>
-      </c>
-      <c r="AA9" s="19" t="s">
-        <v>260</v>
-      </c>
-      <c r="AB9" s="19">
+      <c r="Z10" s="19" t="s">
+        <v>262</v>
+      </c>
+      <c r="AA10" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="AB10" s="19">
         <v>1003.0</v>
       </c>
-      <c r="AC9" s="19">
+      <c r="AC10" s="19">
         <v>50.0</v>
       </c>
-      <c r="AD9" s="19">
+      <c r="AD10" s="19">
         <v>150.0</v>
       </c>
-      <c r="AE9" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="AF9" s="19" t="s">
-        <v>261</v>
-      </c>
-      <c r="AG9" s="19" t="s">
-        <v>262</v>
-      </c>
-      <c r="AH9" s="19" t="s">
-        <v>263</v>
-      </c>
-      <c r="AI9" s="19" t="s">
+      <c r="AE10" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="AF10" s="19" t="s">
         <v>264</v>
       </c>
-      <c r="AJ9" s="19" t="s">
+      <c r="AG10" s="19" t="s">
         <v>265</v>
       </c>
-      <c r="AK9" s="52">
+      <c r="AH10" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="AI10" s="19" t="s">
+        <v>267</v>
+      </c>
+      <c r="AJ10" s="19" t="s">
+        <v>268</v>
+      </c>
+      <c r="AK10" s="52">
         <v>43101.0</v>
       </c>
-      <c r="AL9" s="19">
+      <c r="AL10" s="19">
         <v>40000.0</v>
       </c>
-      <c r="AM9" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="AN9" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="AO9" s="52">
+      <c r="AM10" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="AN10" s="19" t="s">
+        <v>269</v>
+      </c>
+      <c r="AO10" s="52">
         <v>43831.0</v>
       </c>
-      <c r="AP9" s="19">
+      <c r="AP10" s="19">
         <v>40000.0</v>
       </c>
-      <c r="AQ9" s="19" t="s">
-        <v>230</v>
-      </c>
-      <c r="AR9" s="19" t="s">
-        <v>230</v>
-      </c>
-      <c r="AS9" s="19" t="s">
-        <v>230</v>
-      </c>
-      <c r="AT9" s="49" t="str">
+      <c r="AQ10" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="AR10" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="AS10" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="AT10" s="49" t="str">
         <f t="shared" si="2"/>
         <v>EQU.RT.EQU.001.MAJ.01.........</v>
       </c>
-      <c r="AU9" s="19" t="s">
-        <v>230</v>
-      </c>
-      <c r="AV9" s="19" t="s">
-        <v>230</v>
-      </c>
-      <c r="AW9" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="AX9" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="AY9" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="AZ9" s="51" t="s">
-        <v>231</v>
-      </c>
-      <c r="BA9" s="19">
+      <c r="AU10" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="AV10" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="AW10" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="AX10" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="AY10" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="AZ10" s="51" t="s">
+        <v>234</v>
+      </c>
+      <c r="BA10" s="19">
         <v>220000.0</v>
       </c>
-      <c r="BB9" s="52">
+      <c r="BB10" s="52">
         <v>47484.0</v>
       </c>
-      <c r="BC9" s="19">
+      <c r="BC10" s="19">
         <v>4000000.0</v>
       </c>
-      <c r="BD9" s="19" t="s">
-        <v>229</v>
-      </c>
-      <c r="BE9" s="19">
+      <c r="BD10" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="BE10" s="19">
         <v>3.0</v>
       </c>
-      <c r="BF9" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="BG9" s="52">
+      <c r="BF10" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="BG10" s="52">
         <v>43831.0</v>
       </c>
-      <c r="BH9" s="25" t="s">
-        <v>232</v>
-      </c>
-      <c r="BI9" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="BJ9" s="19">
+      <c r="BH10" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="BI10" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="BJ10" s="19">
         <v>1003.0</v>
       </c>
-      <c r="BK9" s="19" t="s">
-        <v>267</v>
-      </c>
-      <c r="BL9" s="50" t="s">
-        <v>231</v>
-      </c>
-      <c r="BM9" s="50" t="s">
-        <v>231</v>
-      </c>
-      <c r="BN9" s="50" t="s">
+      <c r="BK10" s="19" t="s">
+        <v>270</v>
+      </c>
+      <c r="BL10" s="50" t="s">
         <v>234</v>
       </c>
-      <c r="BO9" s="50" t="s">
+      <c r="BM10" s="50" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="43" t="s">
-        <v>268</v>
-      </c>
-      <c r="B10" s="21">
-        <v>1002.0</v>
-      </c>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="54" t="s">
-        <v>217</v>
-      </c>
-      <c r="G10" s="54" t="s">
-        <v>217</v>
-      </c>
-      <c r="H10" s="54" t="s">
-        <v>217</v>
-      </c>
-      <c r="I10" s="54" t="s">
-        <v>217</v>
-      </c>
-      <c r="J10" s="54" t="s">
-        <v>217</v>
-      </c>
-      <c r="K10" s="54" t="s">
-        <v>217</v>
-      </c>
-      <c r="L10" s="54" t="s">
-        <v>217</v>
-      </c>
-      <c r="M10" s="54" t="s">
-        <v>217</v>
-      </c>
-      <c r="N10" s="54" t="s">
-        <v>217</v>
-      </c>
-      <c r="O10" s="53"/>
-      <c r="P10" s="54" t="s">
-        <v>217</v>
-      </c>
-      <c r="Q10" s="54" t="s">
-        <v>217</v>
-      </c>
-      <c r="R10" s="54" t="s">
-        <v>217</v>
-      </c>
-      <c r="S10" s="53"/>
-      <c r="T10" s="53"/>
-      <c r="U10" s="53"/>
-      <c r="V10" s="53"/>
-      <c r="W10" s="53"/>
-      <c r="X10" s="53"/>
-      <c r="Y10" s="53"/>
-      <c r="Z10" s="53"/>
-      <c r="AA10" s="53"/>
-      <c r="AB10" s="53"/>
-      <c r="AC10" s="53"/>
-      <c r="AD10" s="53"/>
-      <c r="AE10" s="53"/>
-      <c r="AF10" s="53"/>
-      <c r="AG10" s="53"/>
-      <c r="AH10" s="53"/>
-      <c r="AI10" s="53"/>
-      <c r="AJ10" s="53"/>
-      <c r="AK10" s="53"/>
-      <c r="AL10" s="53"/>
-      <c r="AM10" s="55" t="s">
-        <v>217</v>
-      </c>
-      <c r="AN10" s="53"/>
-      <c r="AO10" s="53"/>
-      <c r="AP10" s="53"/>
-      <c r="AQ10" s="53"/>
-      <c r="AR10" s="53"/>
-      <c r="AS10" s="53"/>
-      <c r="AT10" s="53"/>
-      <c r="AU10" s="53"/>
-      <c r="AV10" s="53"/>
-      <c r="AW10" s="55" t="s">
-        <v>217</v>
-      </c>
-      <c r="AX10" s="55" t="s">
-        <v>217</v>
-      </c>
-      <c r="AY10" s="55" t="s">
-        <v>217</v>
-      </c>
-      <c r="AZ10" s="54"/>
-      <c r="BA10" s="53"/>
-      <c r="BB10" s="53"/>
-      <c r="BC10" s="53"/>
-      <c r="BD10" s="53"/>
-      <c r="BE10" s="53"/>
-      <c r="BF10" s="55" t="s">
-        <v>217</v>
-      </c>
-      <c r="BG10" s="53"/>
-      <c r="BH10" s="53"/>
-      <c r="BI10" s="55" t="s">
-        <v>217</v>
-      </c>
-      <c r="BJ10" s="53"/>
-      <c r="BK10" s="53"/>
-      <c r="BL10" s="54"/>
-      <c r="BM10" s="54"/>
-      <c r="BN10" s="54"/>
-      <c r="BO10" s="54"/>
+      <c r="BN10" s="50" t="s">
+        <v>237</v>
+      </c>
+      <c r="BO10" s="50" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="43" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B11" s="21">
-        <v>1003.0</v>
+        <v>1002.0</v>
       </c>
       <c r="C11" s="53"/>
       <c r="D11" s="53"/>
       <c r="E11" s="53"/>
-      <c r="F11" s="54" t="s">
-        <v>217</v>
-      </c>
-      <c r="G11" s="54" t="s">
-        <v>217</v>
-      </c>
-      <c r="H11" s="54" t="s">
-        <v>217</v>
-      </c>
-      <c r="I11" s="54" t="s">
-        <v>217</v>
-      </c>
-      <c r="J11" s="54" t="s">
-        <v>217</v>
-      </c>
-      <c r="K11" s="54" t="s">
-        <v>217</v>
-      </c>
-      <c r="L11" s="54" t="s">
-        <v>217</v>
-      </c>
-      <c r="M11" s="54" t="s">
-        <v>217</v>
-      </c>
-      <c r="N11" s="54" t="s">
-        <v>217</v>
-      </c>
+      <c r="F11" s="54"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="54"/>
+      <c r="I11" s="54"/>
+      <c r="J11" s="54"/>
+      <c r="K11" s="54"/>
+      <c r="L11" s="54"/>
+      <c r="M11" s="54"/>
+      <c r="N11" s="54"/>
       <c r="O11" s="53"/>
-      <c r="P11" s="54" t="s">
-        <v>217</v>
-      </c>
-      <c r="Q11" s="54" t="s">
-        <v>217</v>
-      </c>
-      <c r="R11" s="54" t="s">
-        <v>217</v>
-      </c>
+      <c r="P11" s="54"/>
+      <c r="Q11" s="54"/>
+      <c r="R11" s="54"/>
       <c r="S11" s="53"/>
       <c r="T11" s="53"/>
       <c r="U11" s="53"/>
@@ -7114,9 +7063,7 @@
       <c r="AJ11" s="53"/>
       <c r="AK11" s="53"/>
       <c r="AL11" s="53"/>
-      <c r="AM11" s="55" t="s">
-        <v>217</v>
-      </c>
+      <c r="AM11" s="55"/>
       <c r="AN11" s="53"/>
       <c r="AO11" s="53"/>
       <c r="AP11" s="53"/>
@@ -7126,29 +7073,19 @@
       <c r="AT11" s="53"/>
       <c r="AU11" s="53"/>
       <c r="AV11" s="53"/>
-      <c r="AW11" s="55" t="s">
-        <v>217</v>
-      </c>
-      <c r="AX11" s="55" t="s">
-        <v>217</v>
-      </c>
-      <c r="AY11" s="55" t="s">
-        <v>217</v>
-      </c>
+      <c r="AW11" s="55"/>
+      <c r="AX11" s="55"/>
+      <c r="AY11" s="55"/>
       <c r="AZ11" s="54"/>
       <c r="BA11" s="53"/>
       <c r="BB11" s="53"/>
       <c r="BC11" s="53"/>
       <c r="BD11" s="53"/>
       <c r="BE11" s="53"/>
-      <c r="BF11" s="55" t="s">
-        <v>217</v>
-      </c>
+      <c r="BF11" s="55"/>
       <c r="BG11" s="53"/>
       <c r="BH11" s="53"/>
-      <c r="BI11" s="55" t="s">
-        <v>217</v>
-      </c>
+      <c r="BI11" s="55"/>
       <c r="BJ11" s="53"/>
       <c r="BK11" s="53"/>
       <c r="BL11" s="54"/>
@@ -7157,8 +7094,12 @@
       <c r="BO11" s="54"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="43"/>
-      <c r="B12" s="44"/>
+      <c r="A12" s="43" t="s">
+        <v>272</v>
+      </c>
+      <c r="B12" s="21">
+        <v>1003.0</v>
+      </c>
       <c r="C12" s="53"/>
       <c r="D12" s="53"/>
       <c r="E12" s="53"/>
@@ -7364,11 +7305,73 @@
       <c r="BO14" s="54"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="56"/>
-      <c r="B15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="49"/>
-      <c r="J15" s="49"/>
+      <c r="A15" s="43"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="54"/>
+      <c r="G15" s="54"/>
+      <c r="H15" s="54"/>
+      <c r="I15" s="54"/>
+      <c r="J15" s="54"/>
+      <c r="K15" s="54"/>
+      <c r="L15" s="54"/>
+      <c r="M15" s="54"/>
+      <c r="N15" s="54"/>
+      <c r="O15" s="53"/>
+      <c r="P15" s="54"/>
+      <c r="Q15" s="54"/>
+      <c r="R15" s="54"/>
+      <c r="S15" s="53"/>
+      <c r="T15" s="53"/>
+      <c r="U15" s="53"/>
+      <c r="V15" s="53"/>
+      <c r="W15" s="53"/>
+      <c r="X15" s="53"/>
+      <c r="Y15" s="53"/>
+      <c r="Z15" s="53"/>
+      <c r="AA15" s="53"/>
+      <c r="AB15" s="53"/>
+      <c r="AC15" s="53"/>
+      <c r="AD15" s="53"/>
+      <c r="AE15" s="53"/>
+      <c r="AF15" s="53"/>
+      <c r="AG15" s="53"/>
+      <c r="AH15" s="53"/>
+      <c r="AI15" s="53"/>
+      <c r="AJ15" s="53"/>
+      <c r="AK15" s="53"/>
+      <c r="AL15" s="53"/>
+      <c r="AM15" s="55"/>
+      <c r="AN15" s="53"/>
+      <c r="AO15" s="53"/>
+      <c r="AP15" s="53"/>
+      <c r="AQ15" s="53"/>
+      <c r="AR15" s="53"/>
+      <c r="AS15" s="53"/>
+      <c r="AT15" s="53"/>
+      <c r="AU15" s="53"/>
+      <c r="AV15" s="53"/>
+      <c r="AW15" s="55"/>
+      <c r="AX15" s="55"/>
+      <c r="AY15" s="55"/>
+      <c r="AZ15" s="54"/>
+      <c r="BA15" s="53"/>
+      <c r="BB15" s="53"/>
+      <c r="BC15" s="53"/>
+      <c r="BD15" s="53"/>
+      <c r="BE15" s="53"/>
+      <c r="BF15" s="55"/>
+      <c r="BG15" s="53"/>
+      <c r="BH15" s="53"/>
+      <c r="BI15" s="55"/>
+      <c r="BJ15" s="53"/>
+      <c r="BK15" s="53"/>
+      <c r="BL15" s="54"/>
+      <c r="BM15" s="54"/>
+      <c r="BN15" s="54"/>
+      <c r="BO15" s="54"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="56"/>
@@ -8806,6 +8809,7 @@
       <c r="J220" s="49"/>
     </row>
     <row r="221" ht="15.75" customHeight="1">
+      <c r="A221" s="56"/>
       <c r="B221" s="49"/>
       <c r="F221" s="49"/>
       <c r="G221" s="49"/>
@@ -13484,6 +13488,12 @@
       <c r="F1000" s="49"/>
       <c r="G1000" s="49"/>
       <c r="J1000" s="49"/>
+    </row>
+    <row r="1001" ht="15.75" customHeight="1">
+      <c r="B1001" s="49"/>
+      <c r="F1001" s="49"/>
+      <c r="G1001" s="49"/>
+      <c r="J1001" s="49"/>
     </row>
   </sheetData>
   <printOptions/>
@@ -13572,7 +13582,7 @@
     </row>
     <row r="4">
       <c r="A4" s="59" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B4" s="61"/>
       <c r="C4" s="60"/>
@@ -13581,7 +13591,7 @@
     </row>
     <row r="5">
       <c r="A5" s="59" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B5" s="61"/>
       <c r="C5" s="60"/>
@@ -13590,7 +13600,7 @@
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="62" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B6" s="63"/>
       <c r="C6" s="64"/>
@@ -15046,7 +15056,7 @@
     <col customWidth="1" min="1" max="1" width="31.88"/>
     <col customWidth="1" min="2" max="2" width="20.75"/>
     <col customWidth="1" min="3" max="3" width="9.13"/>
-    <col customWidth="1" min="4" max="4" width="19.63"/>
+    <col customWidth="1" min="4" max="4" width="31.0"/>
     <col customWidth="1" min="5" max="5" width="12.63"/>
     <col customWidth="1" min="6" max="6" width="19.0"/>
   </cols>
@@ -15098,7 +15108,7 @@
       <c r="B2" s="59"/>
       <c r="C2" s="65"/>
       <c r="D2" s="65" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="E2" s="60"/>
       <c r="F2" s="60"/>
@@ -15115,7 +15125,7 @@
     </row>
     <row r="4">
       <c r="A4" s="59" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B4" s="61"/>
       <c r="C4" s="60"/>
@@ -15125,19 +15135,19 @@
     </row>
     <row r="5">
       <c r="A5" s="59" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B5" s="61"/>
       <c r="C5" s="60"/>
       <c r="D5" s="65" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="E5" s="60"/>
       <c r="F5" s="60"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="62" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B6" s="63"/>
       <c r="C6" s="64"/>
@@ -15147,99 +15157,103 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="43" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="B7" s="19">
         <v>1004.0</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="E7" s="19">
         <v>10.0</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="43" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="B8" s="19">
         <v>1004.0</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="E8" s="19">
         <v>20.0</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="43" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="B9" s="19">
         <v>1004.0</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="E9" s="19">
         <v>30.0</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="43" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="B10" s="19">
         <v>1004.0</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="E10" s="19">
         <v>40.0</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="43" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="B11" s="19">
         <v>1004.0</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>275</v>
-      </c>
-      <c r="E11" s="66"/>
-      <c r="F11" s="66"/>
+        <v>278</v>
+      </c>
+      <c r="E11" s="66" t="s">
+        <v>220</v>
+      </c>
+      <c r="F11" s="66" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="56"/>
@@ -16728,56 +16742,56 @@
     </row>
     <row r="4">
       <c r="A4" s="59" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B4" s="59"/>
       <c r="C4" s="60"/>
     </row>
     <row r="5">
       <c r="A5" s="59" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B5" s="61"/>
       <c r="C5" s="65"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="62" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B6" s="63"/>
       <c r="C6" s="64"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="43" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="B7" s="46" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="43" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="B8" s="46" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="43" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="B9" s="46" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
@@ -18213,13 +18227,13 @@
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
       <c r="A1" s="67" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="B1" s="68" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="C1" s="68" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1"/>
@@ -19253,7 +19267,7 @@
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="36"/>
       <c r="B1" s="38" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="C1" s="38"/>
       <c r="D1" s="38"/>
@@ -19294,19 +19308,19 @@
     </row>
     <row r="4">
       <c r="A4" s="40" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B4" s="40"/>
     </row>
     <row r="5">
       <c r="A5" s="40" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B5" s="40"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="42" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B6" s="42"/>
     </row>

</xml_diff>

<commit_message>
AJOUT de JDDKW 'TBD'
en remplacement des valeurs de type 'ATTENTE REPONSE MOE'
</commit_message>
<xml_diff>
--- a/TNR_JDD/JDD.RT.EQU.xlsx
+++ b/TNR_JDD/JDD.RT.EQU.xlsx
@@ -114,7 +114,7 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mjK/gRnrXUkH4k+J4VcGz9/gtmp+w=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7miIvsDjd9C4mQmkioo0ARY2enGbiw=="/>
     </ext>
   </extLst>
 </comments>
@@ -825,7 +825,7 @@
     <t>EQU.RT.EQU.001.CRE.01</t>
   </si>
   <si>
-    <t>ATTENTE REPONSE MOE</t>
+    <t>$TBD</t>
   </si>
   <si>
     <t>PEREETFILS</t>

</xml_diff>